<commit_message>
Updated files for 7/8/25
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysAdd.xlsx
+++ b/Pathways Update/PathwaysAdd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Marble</t>
+          <t>Trivento</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>57806699</t>
+          <t>58448688</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -498,42 +498,42 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cat Adoption Room G</t>
+          <t>Cat Adoption Condo Rooms</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>04/28/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2y 3m 17d</t>
+          <t>2y 2m 1d</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Hold - Behavior Mod.</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>63</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FRANKLIN</t>
+          <t>CHATEAU ST. MICHELLE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>58365909</t>
+          <t>58459452</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -543,42 +543,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Cat Adoption Condo Rooms</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>04/29/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>8y 2m 6d</t>
+          <t>3y 2m 0d</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>Hold - Behavior Mod.</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>61.8</v>
+        <v>60.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PLUM</t>
+          <t>BEATRICE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>58377570</t>
+          <t>58442198</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -588,42 +588,42 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>04/25/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Domestic Longhair</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>7y 2m 4d</t>
+          <t>2y 2m 1d</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>65.7</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mochi</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>58353916</t>
+          <t>58444073</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -633,267 +633,263 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Offsite Adoptions</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>04/22/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Domestic Longhair</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2m 29d</t>
+          <t>3m 0d</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>68.7</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CARAMEL</t>
+          <t>Masie</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>58640671</t>
+          <t>58450156</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Adoptions Office (Jill's) #152</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>06/04/2025</t>
+          <t>05/07/2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>5y 1m 15d</t>
+          <t>1y 8m 1d</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Hold - Behavior Mod.</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>25.8</v>
+        <v>61.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SUDS</t>
+          <t>Quinta Nova</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>58598619</t>
+          <t>58454445</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Dog Adoptions A</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>05/29/2025</t>
+          <t>05/07/2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Chihuahua, Short Coat</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5y 1m 1d</t>
+          <t>2y 2m 1d</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Available - Behind the Scenes</t>
+          <t>In If the Fur Fits - Behavior</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>31.8</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Momo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>58604196</t>
+          <t>58448506</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dog Adoptions A</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>05/30/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Ragdoll</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>5y 1m 0d</t>
+          <t>4m 12d</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Available - Behind the Scenes</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>31</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Benji</t>
+          <t>Elvis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>58639325</t>
+          <t>58452209</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dog Adoptions A</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>06/04/2025</t>
+          <t>05/07/2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10y 26d</t>
+          <t>1y 2m 1d</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Available - Behind the Scenes</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>25.8</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Pancake</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>58596028</t>
+          <t>58447679</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dog Adoptions B</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>06/05/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
+          <t>Snowshoe</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3y 25d</t>
+          <t>3m 7d</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>24.9</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Snow Cone</t>
+          <t>Missy</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>58640624</t>
+          <t>58764565</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -903,42 +899,42 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dog Adoptions C</t>
+          <t>Dog Adoptions B</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>06/04/2025</t>
+          <t>06/23/2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>5y 1m 6d</t>
+          <t>3y 14d</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Hold - Meet and Greet</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>25.8</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Goldie</t>
+          <t>Karma</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>58622481</t>
+          <t>58764550</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -948,12 +944,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dog Adoptions C</t>
+          <t>Dog Adoptions B</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>06/02/2025</t>
+          <t>06/23/2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -963,27 +959,27 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7y 6m 19d</t>
+          <t>2y 15d</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Hold - Meet and Greet</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>27.8</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Beau</t>
+          <t>Onyx</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>58677023</t>
+          <t>58622436</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -993,42 +989,42 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dog Adoptions C</t>
+          <t>Dog Adoptions D</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>06/10/2025</t>
+          <t>06/21/2025</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Shepherd</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2y 20d</t>
+          <t>6y 1m 6d</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Available - ITFF Behavior</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>19.9</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Maya</t>
+          <t>CINDER</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>58703260</t>
+          <t>58753979</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1043,7 +1039,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>06/13/2025</t>
+          <t>06/20/2025</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1053,27 +1049,27 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11y 17d</t>
+          <t>10y 4m 10d</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Hold - Doc</t>
+          <t>Hold - Rescue</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>16.9</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Iris</t>
+          <t>Diamond</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>58545411</t>
+          <t>57957792</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1083,12 +1079,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>Dog Holding F</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>05/27/2025</t>
+          <t>03/04/2025</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1098,27 +1094,27 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10m 2d</t>
+          <t>1y 1m 26d</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>In Foster</t>
+          <t>Hold - Behavior</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>33.9</v>
+        <v>125.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Pickley</t>
+          <t>EASTON</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>58605268</t>
+          <t>58718199</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1128,42 +1124,42 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>05/31/2025</t>
+          <t>06/18/2025</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Poodle, Standard</t>
+          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>4y 1m 0d</t>
+          <t>8y 2m 0d</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>In SAFE Foster</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>29.9</v>
+        <v>19.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>THOR</t>
+          <t>Magnus</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>32144299</t>
+          <t>58690617</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1178,37 +1174,37 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>06/09/2025</t>
+          <t>06/19/2025</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Collie, Smooth</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>9y 5m 17d</t>
+          <t>4y 27d</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>20.8</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bubba</t>
+          <t>JEWELIE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>57976477</t>
+          <t>58753970</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1223,172 +1219,168 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>06/06/2025</t>
+          <t>06/20/2025</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Mixed Breed, Small (under 24 lbs fully grown)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>11m 23d</t>
+          <t>10y 17d</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>24</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t>FIREFLY</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>58597214</t>
+          <t>58695418</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Rabbit</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Cat Adoption Condo Rooms</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>06/03/2025</t>
+          <t>06/20/2025</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>5y 1m 1d</t>
-        </is>
-      </c>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>26.9</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RAYNE</t>
+          <t>Luna</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>57710656</t>
+          <t>58744079</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Donkey</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Farm</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>06/13/2025</t>
+          <t>06/17/2025</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Miniature Donkey</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>4y 5m 6d</t>
+          <t>15y 19d</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Trial</t>
+          <t>Hold - Doc</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>16.8</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HEATH</t>
+          <t>Moose</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>58654173</t>
+          <t>58728965</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Farm Type Fowl</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Farm</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>06/06/2025</t>
+          <t>06/17/2025</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Whippet</t>
+          <t>Chicken</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>7m 26d</t>
+          <t>8m 23d</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Trial</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>23.9</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MARINA</t>
+          <t>FUZZY SLIPPER</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>58706705</t>
+          <t>58757630</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1398,79 +1390,87 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Adoptions Lobby</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>06/13/2025</t>
+          <t>06/21/2025</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>Mini-Lop</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2m 29d</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>In Foster</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FLIP FLOP</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>58757640</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Rabbit</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Foster Home</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>06/21/2025</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>Rex</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Available</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>58654136</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Domestic (Cage) Bird</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Farm</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>06/06/2025</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Quail, Japanese</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3m 3d</t>
+          <t>2m 29d</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>23.9</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bunny 2</t>
+          <t>Leonardo</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>58212975</t>
+          <t>58764920</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1485,17 +1485,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>03/30/2025</t>
+          <t>06/23/2025</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Florida White</t>
+          <t>Satin</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3m 1d</t>
+          <t>1y 15d</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1504,498 +1504,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Bunny 1</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>58212978</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Florida White</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Glacier</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>58212979</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Florida White</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I26" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Apple</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>58212981</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Florida White</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Cloudy</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>58212982</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Florida White</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I28" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Bunny 5</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>58212985</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Florida White</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I29" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Bunny 7</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>58212987</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Florida White</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I30" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Ham</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>58213029</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Rex</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I31" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Rabbit 1</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>58213031</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Rex</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Rabbit 4</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>58213033</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Rex</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Jam</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>58213035</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Rex</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>91.90000000000001</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>58213036</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>03/30/2025</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Rex</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>3m 1d</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>91.90000000000001</v>
+        <v>14.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update pathways part 1
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysAdd.xlsx
+++ b/Pathways Update/PathwaysAdd.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Trivento</t>
+          <t>MALBEC</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>58448688</t>
+          <t>58520465</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>05/17/2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2y 2m 1d</t>
+          <t>1y 2m 8d</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -522,18 +522,18 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>62.5</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CHATEAU ST. MICHELLE</t>
+          <t>BUCKEYE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>58459452</t>
+          <t>58514522</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -543,42 +543,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cat Adoption Condo Rooms</t>
+          <t>Cat Adoption Room G</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>05/08/2025</t>
+          <t>05/19/2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Domestic Longhair</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3y 2m 0d</t>
+          <t>2y 2m 2d</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Hold - Behavior Mod.</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>60.8</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BEATRICE</t>
+          <t>KATNISS</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>58442198</t>
+          <t>58517968</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>05/16/2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2y 2m 1d</t>
+          <t>3m 3d</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -612,18 +612,18 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>62.8</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>PRIMROSE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>58444073</t>
+          <t>58517971</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>05/16/2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3m 0d</t>
+          <t>3m 3d</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -657,18 +657,18 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>62.8</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Masie</t>
+          <t>HAYMITCH</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>58450156</t>
+          <t>58517973</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -683,17 +683,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>05/07/2025</t>
+          <t>05/16/2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Domestic Longhair</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1y 8m 1d</t>
+          <t>3m 3d</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -702,18 +702,18 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>61.9</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Quinta Nova</t>
+          <t>PEETA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>58454445</t>
+          <t>58517974</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -723,42 +723,42 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>05/07/2025</t>
+          <t>05/16/2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Domestic Longhair</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2y 2m 1d</t>
+          <t>3m 3d</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Behavior</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>61.7</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Momo</t>
+          <t>Sugar</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>58448506</t>
+          <t>58433959</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -768,128 +768,132 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Offsite Adoptions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ragdoll</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4m 12d</t>
+          <t>3m 0d</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>Hold - Adopted!</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>62.6</v>
+        <v>77.59999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Elvis</t>
+          <t>LUNA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>58452209</t>
+          <t>58067302</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Dog</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Dog Adoptions D</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>05/07/2025</t>
+          <t>07/03/2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1y 2m 1d</t>
+          <t>10y 3m 24d</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>Available - Doggie Entourage</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>61.8</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Glow</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>58447679</t>
+          <t>58834563</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Dog</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Dog Holding E</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Snowshoe</t>
+          <t>Bulldog</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3m 7d</t>
+          <t>1y 6m 18d</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Trial</t>
+          <t>Hold - Cruelty Foster</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>62.7</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Missy</t>
+          <t>Katniss</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>58764565</t>
+          <t>58834486</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -899,42 +903,38 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dog Adoptions B</t>
+          <t>Dog Holding E</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>06/23/2025</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>3y 14d</t>
-        </is>
-      </c>
+          <t>Bulldog</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Hold - Meet and Greet</t>
+          <t>Hold - Cruelty Foster</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>14.9</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Karma</t>
+          <t>Sky</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>58764550</t>
+          <t>58854396</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -944,12 +944,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dog Adoptions B</t>
+          <t>Dog Holding F</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>06/23/2025</t>
+          <t>07/07/2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -959,27 +959,27 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2y 15d</t>
+          <t>1y 14d</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Hold - Meet and Greet</t>
+          <t>Hold - For RTO</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>14.9</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Onyx</t>
+          <t>Scruffles</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>58622436</t>
+          <t>58419285</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -989,42 +989,42 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dog Adoptions D</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>06/21/2025</t>
+          <t>05/01/2025</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Shepherd</t>
+          <t>Mixed Breed, Small (under 24 lbs fully grown)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6y 1m 6d</t>
+          <t>15y 2m 19d</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Available - ITFF Behavior</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>16.8</v>
+        <v>81.09999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CINDER</t>
+          <t>Dior</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>58753979</t>
+          <t>58834490</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1034,42 +1034,42 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Dog Holding E</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>06/20/2025</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Bulldog</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>10y 4m 10d</t>
+          <t>1y 18d</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Hold - Rescue</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>17.6</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Diamond</t>
+          <t>Remy</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>57957792</t>
+          <t>58834525</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1079,42 +1079,42 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dog Holding F</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
+          <t>Bulldog, French</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1y 1m 26d</t>
+          <t>1y 17d</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Hold - Behavior</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>125.7</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EASTON</t>
+          <t>Bruno</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>58718199</t>
+          <t>58849570</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1124,42 +1124,42 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>06/18/2025</t>
+          <t>07/05/2025</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>8y 2m 0d</t>
+          <t>5m 16d</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>19.9</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Magnus</t>
+          <t>Lilly</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>58690617</t>
+          <t>58831432</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1174,37 +1174,37 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>06/19/2025</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Chihuahua, Long Coat</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>4y 27d</t>
+          <t>10y 19d</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Trial</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>18.8</v>
+        <v>19.4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>JEWELIE</t>
+          <t>COLT</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>58753970</t>
+          <t>58838875</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1219,292 +1219,112 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>06/20/2025</t>
+          <t>07/07/2025</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Mixed Breed, Small (under 24 lbs fully grown)</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10y 17d</t>
+          <t>10y 13d</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Trial</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>17.6</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>FIREFLY</t>
+          <t>Mabel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>58695418</t>
+          <t>58421981</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Rabbit</t>
+          <t>Dog</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Cat Adoption Condo Rooms</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>06/20/2025</t>
+          <t>07/03/2025</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mix</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
+          <t>Mastiff</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>5m 19d</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>17.8</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Luna</t>
+          <t>SPRITZ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>58744079</t>
+          <t>58831524</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Donkey</t>
+          <t>Rabbit</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Farm</t>
+          <t>Foster Home</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>06/17/2025</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Miniature Donkey</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>15y 19d</t>
-        </is>
-      </c>
+          <t>Holland Lop</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Hold - Doc</t>
+          <t>In Foster</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>20.7</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Moose</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>58728965</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Farm Type Fowl</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Farm</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>06/17/2025</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Chicken</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>8m 23d</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Available</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>20.7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>FUZZY SLIPPER</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>58757630</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>06/21/2025</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Mini-Lop</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2m 29d</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>FLIP FLOP</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>58757640</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>06/21/2025</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Rex</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2m 29d</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Leonardo</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>58764920</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Rabbit</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Foster Home</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>06/23/2025</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Satin</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>1y 15d</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>In Foster</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
-        <v>14.8</v>
+        <v>19.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "update pathways part 1"
This reverts commit d1f5407f5d9eb55d66a5d91f7dc4fc45b079bccc.
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysAdd.xlsx
+++ b/Pathways Update/PathwaysAdd.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MALBEC</t>
+          <t>Trivento</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>58520465</t>
+          <t>58448688</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>05/17/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1y 2m 8d</t>
+          <t>2y 2m 1d</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -522,18 +522,18 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>65.5</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BUCKEYE</t>
+          <t>CHATEAU ST. MICHELLE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>58514522</t>
+          <t>58459452</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -543,42 +543,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cat Adoption Room G</t>
+          <t>Cat Adoption Condo Rooms</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>05/19/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2y 2m 2d</t>
+          <t>3y 2m 0d</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Hold - Behavior Mod.</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>63.5</v>
+        <v>60.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>KATNISS</t>
+          <t>BEATRICE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>58517968</t>
+          <t>58442198</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>05/16/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3m 3d</t>
+          <t>2y 2m 1d</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -612,18 +612,18 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>66.3</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PRIMROSE</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>58517971</t>
+          <t>58444073</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>05/16/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3m 3d</t>
+          <t>3m 0d</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -657,18 +657,18 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>66.3</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HAYMITCH</t>
+          <t>Masie</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>58517973</t>
+          <t>58450156</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -683,17 +683,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>05/16/2025</t>
+          <t>05/07/2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3m 3d</t>
+          <t>1y 8m 1d</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -702,18 +702,18 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>66.3</v>
+        <v>61.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PEETA</t>
+          <t>Quinta Nova</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>58517974</t>
+          <t>58454445</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -723,42 +723,42 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>05/16/2025</t>
+          <t>05/07/2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Domestic Longhair</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3m 3d</t>
+          <t>2y 2m 1d</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>In Foster</t>
+          <t>In If the Fur Fits - Behavior</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>66.3</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sugar</t>
+          <t>Momo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>58433959</t>
+          <t>58448506</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -768,132 +768,128 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Offsite Adoptions</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Domestic Shorthair</t>
+          <t>Ragdoll</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3m 0d</t>
+          <t>4m 12d</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Hold - Adopted!</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>77.59999999999999</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LUNA</t>
+          <t>Elvis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>58067302</t>
+          <t>58452209</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dog Adoptions D</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>07/03/2025</t>
+          <t>05/07/2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Domestic Shorthair</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10y 3m 24d</t>
+          <t>1y 2m 1d</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Available - Doggie Entourage</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>18.5</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Glow</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>58834563</t>
+          <t>58447679</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dog Holding E</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>05/06/2025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Bulldog</t>
+          <t>Snowshoe</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1y 6m 18d</t>
+          <t>3m 7d</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Hold - Cruelty Foster</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>19.2</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Katniss</t>
+          <t>Missy</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>58834486</t>
+          <t>58764565</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -903,38 +899,42 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dog Holding E</t>
+          <t>Dog Adoptions B</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>06/23/2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Bulldog</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>3y 14d</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Hold - Cruelty Foster</t>
+          <t>Hold - Meet and Greet</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>19.2</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Karma</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>58854396</t>
+          <t>58764550</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -944,12 +944,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dog Holding F</t>
+          <t>Dog Adoptions B</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>07/07/2025</t>
+          <t>06/23/2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -959,27 +959,27 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1y 14d</t>
+          <t>2y 15d</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Hold - For RTO</t>
+          <t>Hold - Meet and Greet</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>14.5</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Scruffles</t>
+          <t>Onyx</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>58419285</t>
+          <t>58622436</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -989,42 +989,42 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>Dog Adoptions D</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>05/01/2025</t>
+          <t>06/21/2025</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Mixed Breed, Small (under 24 lbs fully grown)</t>
+          <t>Shepherd</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15y 2m 19d</t>
+          <t>6y 1m 6d</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>In Foster</t>
+          <t>Available - ITFF Behavior</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>81.09999999999999</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dior</t>
+          <t>CINDER</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>58834490</t>
+          <t>58753979</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1034,42 +1034,42 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>Dog Holding E</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>06/20/2025</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Bulldog</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1y 18d</t>
+          <t>10y 4m 10d</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>In Foster</t>
+          <t>Hold - Rescue</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>19.2</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Remy</t>
+          <t>Diamond</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>58834525</t>
+          <t>57957792</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1079,42 +1079,42 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>Dog Holding F</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>03/04/2025</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Bulldog, French</t>
+          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1y 17d</t>
+          <t>1y 1m 26d</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>In Foster</t>
+          <t>Hold - Behavior</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>19.2</v>
+        <v>125.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bruno</t>
+          <t>EASTON</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>58849570</t>
+          <t>58718199</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1124,42 +1124,42 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Foster Home</t>
+          <t>If The Fur Fits</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>07/05/2025</t>
+          <t>06/18/2025</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>5m 16d</t>
+          <t>8y 2m 0d</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>In Foster</t>
+          <t>In If the Fur Fits - Medical</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>16.3</v>
+        <v>19.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lilly</t>
+          <t>Magnus</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>58831432</t>
+          <t>58690617</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1174,37 +1174,37 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>06/19/2025</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Chihuahua, Long Coat</t>
+          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>10y 19d</t>
+          <t>4y 27d</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>19.4</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>COLT</t>
+          <t>JEWELIE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>58838875</t>
+          <t>58753970</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1219,112 +1219,292 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>07/07/2025</t>
+          <t>06/20/2025</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+          <t>Mixed Breed, Small (under 24 lbs fully grown)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10y 13d</t>
+          <t>10y 17d</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Medical</t>
+          <t>In If the Fur Fits - Trial</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>14.5</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mabel</t>
+          <t>FIREFLY</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>58421981</t>
+          <t>58695418</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Rabbit</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>If The Fur Fits</t>
+          <t>Cat Adoption Condo Rooms</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>07/03/2025</t>
+          <t>06/20/2025</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mastiff</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>5m 19d</t>
-        </is>
-      </c>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>In If the Fur Fits - Trial</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>18.5</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SPRITZ</t>
+          <t>Luna</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>58831524</t>
+          <t>58744079</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>Donkey</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Farm</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>06/17/2025</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Miniature Donkey</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>15y 19d</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Hold - Doc</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Moose</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>58728965</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Farm Type Fowl</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Farm</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>06/17/2025</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Chicken</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>8m 23d</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FUZZY SLIPPER</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>58757630</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>Rabbit</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Foster Home</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>07/02/2025</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Holland Lop</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>06/21/2025</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Mini-Lop</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2m 29d</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>In Foster</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>19.4</v>
+      <c r="I22" t="n">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FLIP FLOP</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>58757640</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Rabbit</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Foster Home</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>06/21/2025</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Rex</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2m 29d</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>In Foster</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Leonardo</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>58764920</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Rabbit</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Foster Home</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>06/23/2025</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Satin</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1y 15d</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>In Foster</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>14.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated foster app 8/19 @420
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysAdd.xlsx
+++ b/Pathways Update/PathwaysAdd.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdoptionsFosterMgr\Desktop\SPCAAutomation\Pathways Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383525B7-91A0-40C5-B8D9-D44B67D79918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F46782-1F42-4B44-9427-DC1C9C468D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="690" windowWidth="21600" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="1770" windowWidth="21600" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$9</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -52,103 +52,133 @@
     <t>LOSInDays</t>
   </si>
   <si>
-    <t>Livia</t>
-  </si>
-  <si>
-    <t>58981285</t>
+    <t>SMORES</t>
+  </si>
+  <si>
+    <t>58710884</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Foster Home</t>
+  </si>
+  <si>
+    <t>06/14/2025</t>
+  </si>
+  <si>
+    <t>Domestic Shorthair</t>
+  </si>
+  <si>
+    <t>2y 2m 5d</t>
+  </si>
+  <si>
+    <t>In Foster</t>
+  </si>
+  <si>
+    <t>Petey</t>
+  </si>
+  <si>
+    <t>58804353</t>
   </si>
   <si>
     <t>Dog</t>
   </si>
   <si>
-    <t>Dog Adoptions A</t>
-  </si>
-  <si>
-    <t>07/25/2025</t>
-  </si>
-  <si>
-    <t>Terrier, Pit Bull</t>
-  </si>
-  <si>
-    <t>9y 1m 4d</t>
-  </si>
-  <si>
-    <t>Hold - Behavior</t>
-  </si>
-  <si>
-    <t>Brody</t>
-  </si>
-  <si>
-    <t>58981296</t>
-  </si>
-  <si>
-    <t>2y 3m 19d</t>
-  </si>
-  <si>
-    <t>Hold - Behavior Mod.</t>
-  </si>
-  <si>
-    <t>Karma</t>
-  </si>
-  <si>
-    <t>58955277</t>
-  </si>
-  <si>
-    <t>Dog Adoptions B</t>
-  </si>
-  <si>
-    <t>07/22/2025</t>
-  </si>
-  <si>
-    <t>Mixed Breed, Medium (up to 44 lbs fully grown)</t>
-  </si>
-  <si>
-    <t>1y 8m 10d</t>
+    <t>Dog Adoptions D</t>
+  </si>
+  <si>
+    <t>07/29/2025</t>
+  </si>
+  <si>
+    <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+  </si>
+  <si>
+    <t>11m 22d</t>
   </si>
   <si>
     <t>Available</t>
   </si>
   <si>
-    <t>Polly</t>
-  </si>
-  <si>
-    <t>58981307</t>
-  </si>
-  <si>
-    <t>1y 8m 6d</t>
-  </si>
-  <si>
-    <t>PAISLEE</t>
-  </si>
-  <si>
-    <t>55535513</t>
-  </si>
-  <si>
-    <t>Dog Adoptions D</t>
-  </si>
-  <si>
-    <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
-  </si>
-  <si>
-    <t>5y 4m 25d</t>
-  </si>
-  <si>
-    <t>Evelyn</t>
-  </si>
-  <si>
-    <t>58988867</t>
-  </si>
-  <si>
-    <t>Dog Holding F</t>
-  </si>
-  <si>
-    <t>07/26/2025</t>
-  </si>
-  <si>
-    <t>3y 17d</t>
-  </si>
-  <si>
-    <t>Hold - Doc</t>
+    <t>Remy</t>
+  </si>
+  <si>
+    <t>58959672</t>
+  </si>
+  <si>
+    <t>07/31/2025</t>
+  </si>
+  <si>
+    <t>5y 28d</t>
+  </si>
+  <si>
+    <t>FALCOR</t>
+  </si>
+  <si>
+    <t>58997270</t>
+  </si>
+  <si>
+    <t>Dog Holding E</t>
+  </si>
+  <si>
+    <t>07/30/2025</t>
+  </si>
+  <si>
+    <t>2y 1d</t>
+  </si>
+  <si>
+    <t>Hold - Surgery</t>
+  </si>
+  <si>
+    <t>Graffiti</t>
+  </si>
+  <si>
+    <t>58834498</t>
+  </si>
+  <si>
+    <t>07/02/2025</t>
+  </si>
+  <si>
+    <t>Bulldog</t>
+  </si>
+  <si>
+    <t>1y 1m 16d</t>
+  </si>
+  <si>
+    <t>08/01/2025</t>
+  </si>
+  <si>
+    <t>Farm Type Fowl</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>59024880</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Evaluate</t>
+  </si>
+  <si>
+    <t>59024884</t>
+  </si>
+  <si>
+    <t>KAHLUA</t>
+  </si>
+  <si>
+    <t>58972687</t>
+  </si>
+  <si>
+    <t>Miniature Pig</t>
+  </si>
+  <si>
+    <t>Kune Kune Mini-pig</t>
+  </si>
+  <si>
+    <t>1y 26d</t>
   </si>
 </sst>
 </file>
@@ -511,22 +541,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -585,7 +615,7 @@
         <v>16</v>
       </c>
       <c r="I2">
-        <v>17.8</v>
+        <v>65.8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -596,145 +626,192 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I3">
-        <v>17.8</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
       <c r="I4">
-        <v>20.9</v>
+        <v>18.899999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="I5">
-        <v>17.8</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I6">
-        <v>20.9</v>
+        <v>47.6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7">
-        <v>16.7</v>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>20.9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I7" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated tools for 8.26.25
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysAdd.xlsx
+++ b/Pathways Update/PathwaysAdd.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdoptionsFosterMgr\Desktop\SPCAAutomation\Pathways Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F46782-1F42-4B44-9427-DC1C9C468D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5F8E93-CD60-484A-8FD0-4914113D7830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="1770" windowWidth="21600" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -52,133 +52,199 @@
     <t>LOSInDays</t>
   </si>
   <si>
-    <t>SMORES</t>
-  </si>
-  <si>
-    <t>58710884</t>
+    <t>KIRK</t>
+  </si>
+  <si>
+    <t>58763319</t>
   </si>
   <si>
     <t>Cat</t>
   </si>
   <si>
+    <t>Cat Adoption Condo Rooms</t>
+  </si>
+  <si>
+    <t>06/23/2025</t>
+  </si>
+  <si>
+    <t>Domestic Shorthair</t>
+  </si>
+  <si>
+    <t>4y 2m 3d</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Bella</t>
+  </si>
+  <si>
+    <t>47809430</t>
+  </si>
+  <si>
     <t>Foster Home</t>
   </si>
   <si>
-    <t>06/14/2025</t>
-  </si>
-  <si>
-    <t>Domestic Shorthair</t>
-  </si>
-  <si>
-    <t>2y 2m 5d</t>
+    <t>4y 5m 9d</t>
+  </si>
+  <si>
+    <t>In SAFE Foster</t>
+  </si>
+  <si>
+    <t>PICKLES</t>
+  </si>
+  <si>
+    <t>58729684</t>
+  </si>
+  <si>
+    <t>1y 9m 3d</t>
   </si>
   <si>
     <t>In Foster</t>
   </si>
   <si>
-    <t>Petey</t>
-  </si>
-  <si>
-    <t>58804353</t>
+    <t>Snuggles</t>
+  </si>
+  <si>
+    <t>59066187</t>
   </si>
   <si>
     <t>Dog</t>
   </si>
   <si>
+    <t>Dog Adoptions A</t>
+  </si>
+  <si>
+    <t>08/07/2025</t>
+  </si>
+  <si>
+    <t>Mixed Breed, Small (under 24 lbs fully grown)</t>
+  </si>
+  <si>
+    <t>12y 15d</t>
+  </si>
+  <si>
+    <t>Hold - Doc</t>
+  </si>
+  <si>
+    <t>PANDORA</t>
+  </si>
+  <si>
+    <t>59054823</t>
+  </si>
+  <si>
+    <t>08/06/2025</t>
+  </si>
+  <si>
+    <t>Mastiff</t>
+  </si>
+  <si>
+    <t>4y 20d</t>
+  </si>
+  <si>
+    <t>Hold - Behavior Mod.</t>
+  </si>
+  <si>
+    <t>TIGOR</t>
+  </si>
+  <si>
+    <t>56174456</t>
+  </si>
+  <si>
+    <t>Dog Adoptions C</t>
+  </si>
+  <si>
+    <t>Terrier, American Pit Bull</t>
+  </si>
+  <si>
+    <t>1y 7m 18d</t>
+  </si>
+  <si>
+    <t>HENRY</t>
+  </si>
+  <si>
+    <t>59086932</t>
+  </si>
+  <si>
+    <t>08/11/2025</t>
+  </si>
+  <si>
+    <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
+  </si>
+  <si>
+    <t>1y 15d</t>
+  </si>
+  <si>
+    <t>Clementine</t>
+  </si>
+  <si>
+    <t>59007999</t>
+  </si>
+  <si>
+    <t>08/01/2025</t>
+  </si>
+  <si>
+    <t>1y 27d</t>
+  </si>
+  <si>
+    <t>Kash</t>
+  </si>
+  <si>
+    <t>59088015</t>
+  </si>
+  <si>
     <t>Dog Adoptions D</t>
   </si>
   <si>
-    <t>07/29/2025</t>
-  </si>
-  <si>
-    <t>Mixed Breed, Large (over 44 lbs fully grown)</t>
-  </si>
-  <si>
-    <t>11m 22d</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Remy</t>
-  </si>
-  <si>
-    <t>58959672</t>
-  </si>
-  <si>
-    <t>07/31/2025</t>
-  </si>
-  <si>
-    <t>5y 28d</t>
-  </si>
-  <si>
-    <t>FALCOR</t>
-  </si>
-  <si>
-    <t>58997270</t>
+    <t>Akita</t>
+  </si>
+  <si>
+    <t>2y 15d</t>
+  </si>
+  <si>
+    <t>Hold - Meet and Greet</t>
+  </si>
+  <si>
+    <t>KOODA</t>
+  </si>
+  <si>
+    <t>59063506</t>
   </si>
   <si>
     <t>Dog Holding E</t>
   </si>
   <si>
-    <t>07/30/2025</t>
-  </si>
-  <si>
-    <t>2y 1d</t>
+    <t>Shiba Inu</t>
+  </si>
+  <si>
+    <t>8y 19d</t>
   </si>
   <si>
     <t>Hold - Surgery</t>
   </si>
   <si>
-    <t>Graffiti</t>
-  </si>
-  <si>
-    <t>58834498</t>
-  </si>
-  <si>
-    <t>07/02/2025</t>
-  </si>
-  <si>
-    <t>Bulldog</t>
-  </si>
-  <si>
-    <t>1y 1m 16d</t>
-  </si>
-  <si>
-    <t>08/01/2025</t>
-  </si>
-  <si>
-    <t>Farm Type Fowl</t>
-  </si>
-  <si>
-    <t>Farm</t>
-  </si>
-  <si>
-    <t>59024880</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Evaluate</t>
-  </si>
-  <si>
-    <t>59024884</t>
-  </si>
-  <si>
-    <t>KAHLUA</t>
-  </si>
-  <si>
-    <t>58972687</t>
-  </si>
-  <si>
-    <t>Miniature Pig</t>
-  </si>
-  <si>
-    <t>Kune Kune Mini-pig</t>
-  </si>
-  <si>
-    <t>1y 26d</t>
+    <t>Zane</t>
+  </si>
+  <si>
+    <t>59013434</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>59077128</t>
+  </si>
+  <si>
+    <t>Dog Holding F</t>
+  </si>
+  <si>
+    <t>08/09/2025</t>
+  </si>
+  <si>
+    <t>German Shepherd</t>
+  </si>
+  <si>
+    <t>4y 12d</t>
   </si>
 </sst>
 </file>
@@ -541,21 +607,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -615,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="I2">
-        <v>65.8</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -626,192 +692,319 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
       <c r="I3">
-        <v>20.9</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
       <c r="I4">
-        <v>18.899999999999999</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
       <c r="I5">
-        <v>19.899999999999999</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
       <c r="I6">
-        <v>47.6</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
         <v>44</v>
       </c>
       <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="I7">
-        <v>17.899999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I8">
-        <v>17.899999999999999</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I9">
-        <v>20.9</v>
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13">
+        <v>16.899999999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I13" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>